<commit_message>
Update figures with new data
</commit_message>
<xml_diff>
--- a/data/3-analysis/output-results/tables/institution-median-rep-2023-11-28.xlsx
+++ b/data/3-analysis/output-results/tables/institution-median-rep-2023-11-28.xlsx
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="B12">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="C12">
         <v>602</v>
@@ -696,354 +696,354 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Oslo University Hospital</t>
+          <t>Örebro University</t>
         </is>
       </c>
       <c r="B27">
-        <v>740</v>
+        <v>981</v>
       </c>
       <c r="C27">
-        <v>1057</v>
+        <v>917</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Oulu University Hospital</t>
+          <t>Örebro University Hospital</t>
         </is>
       </c>
       <c r="B28">
-        <v>1213</v>
+        <v>182</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Sahlgrenska University Hospital</t>
+          <t>Oslo University Hospital</t>
         </is>
       </c>
       <c r="B29">
-        <v>867</v>
+        <v>740</v>
       </c>
       <c r="C29">
-        <v>1201</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Skane University Hospital</t>
+          <t>Oulu University Hospital</t>
         </is>
       </c>
       <c r="B30">
-        <v>523</v>
-      </c>
-      <c r="C30">
-        <v>1119</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>St. Olav’s University Hospital</t>
+          <t>Sahlgrenska University Hospital</t>
         </is>
       </c>
       <c r="B31">
-        <v>1331</v>
+        <v>867</v>
+      </c>
+      <c r="C31">
+        <v>1201</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Steno Diabetes Center Copenhagen</t>
+          <t>Skane University Hospital</t>
         </is>
       </c>
       <c r="B32">
-        <v>560</v>
+        <v>523</v>
       </c>
       <c r="C32">
-        <v>408.0000000000001</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Stockholm South General Hospital</t>
+          <t>St. Olav’s University Hospital</t>
         </is>
       </c>
       <c r="B33">
-        <v>216</v>
-      </c>
-      <c r="C33">
-        <v>1052</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Tampere University Hospital</t>
+          <t>Steno Diabetes Center Copenhagen</t>
         </is>
       </c>
       <c r="B34">
-        <v>400.5000000000001</v>
+        <v>560</v>
       </c>
       <c r="C34">
-        <v>734.0000000000001</v>
+        <v>408.0000000000001</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>The National University Hospital of Iceland</t>
+          <t>Stockholm South General Hospital</t>
         </is>
       </c>
       <c r="B35">
-        <v>992</v>
+        <v>216</v>
       </c>
       <c r="C35">
-        <v>765.9999999999999</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Turku University Hospital</t>
+          <t>Tampere University Hospital</t>
         </is>
       </c>
       <c r="B36">
-        <v>913</v>
+        <v>400.5000000000001</v>
+      </c>
+      <c r="C36">
+        <v>734.0000000000001</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>UiT The Arctic University of Norway</t>
+          <t>The National University Hospital of Iceland</t>
         </is>
       </c>
       <c r="B37">
-        <v>655.4999999999999</v>
+        <v>992</v>
+      </c>
+      <c r="C37">
+        <v>765.9999999999999</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Umeå University</t>
+          <t>Turku University Hospital</t>
         </is>
       </c>
       <c r="B38">
-        <v>909.9999999999999</v>
+        <v>913</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>University Hospital of North Norway</t>
+          <t>UiT The Arctic University of Norway</t>
         </is>
       </c>
       <c r="B39">
-        <v>973</v>
+        <v>655.4999999999999</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>University Hospital of Umeå</t>
+          <t>Umeå University</t>
         </is>
       </c>
       <c r="B40">
-        <v>427</v>
-      </c>
-      <c r="C40">
-        <v>609.9999999999999</v>
+        <v>909.9999999999999</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>University of Bergen</t>
+          <t>University Hospital of North Norway</t>
         </is>
       </c>
       <c r="B41">
-        <v>689</v>
+        <v>973</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>University of Copenhagen</t>
+          <t>University Hospital of Umeå</t>
         </is>
       </c>
       <c r="B42">
-        <v>846</v>
+        <v>427</v>
       </c>
       <c r="C42">
-        <v>1220</v>
+        <v>609.9999999999999</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>University of Eastern Finland</t>
+          <t>University of Bergen</t>
         </is>
       </c>
       <c r="B43">
-        <v>1278</v>
-      </c>
-      <c r="C43">
-        <v>1292</v>
+        <v>689</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>University of Helsinki</t>
+          <t>University of Copenhagen</t>
         </is>
       </c>
       <c r="B44">
-        <v>723</v>
+        <v>846</v>
       </c>
       <c r="C44">
-        <v>1163</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>University of Iceland</t>
+          <t>University of Eastern Finland</t>
         </is>
       </c>
       <c r="B45">
-        <v>1306</v>
+        <v>1278</v>
       </c>
       <c r="C45">
-        <v>828.9999999999998</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>University of Oslo</t>
+          <t>University of Helsinki</t>
         </is>
       </c>
       <c r="B46">
-        <v>670</v>
+        <v>723</v>
       </c>
       <c r="C46">
-        <v>566</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>University of Oulu</t>
+          <t>University of Iceland</t>
         </is>
       </c>
       <c r="B47">
-        <v>1191</v>
+        <v>1306</v>
       </c>
       <c r="C47">
-        <v>1832</v>
+        <v>828.9999999999998</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>University of Southern Denmark</t>
+          <t>University of Oslo</t>
         </is>
       </c>
       <c r="B48">
-        <v>577.4999999999999</v>
+        <v>670</v>
       </c>
       <c r="C48">
-        <v>510.9999999999999</v>
+        <v>566</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>University of Tampere</t>
+          <t>University of Oulu</t>
         </is>
       </c>
       <c r="B49">
-        <v>276</v>
+        <v>1191</v>
       </c>
       <c r="C49">
-        <v>701.9999999999999</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>University of Turku</t>
+          <t>University of Southern Denmark</t>
         </is>
       </c>
       <c r="B50">
-        <v>759</v>
+        <v>577.4999999999999</v>
       </c>
       <c r="C50">
-        <v>1194.5</v>
+        <v>510.9999999999999</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Uppsala Academic Hospital</t>
+          <t>University of Tampere</t>
         </is>
       </c>
       <c r="B51">
-        <v>948.9999999999999</v>
+        <v>276</v>
       </c>
       <c r="C51">
-        <v>594.9999999999999</v>
+        <v>701.9999999999999</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Uppsala University</t>
+          <t>University of Turku</t>
         </is>
       </c>
       <c r="B52">
-        <v>971</v>
+        <v>759</v>
+      </c>
+      <c r="C52">
+        <v>1194.5</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Zealand University Hospital</t>
+          <t>Uppsala Academic Hospital</t>
         </is>
       </c>
       <c r="B53">
-        <v>593.5</v>
+        <v>948.9999999999999</v>
       </c>
       <c r="C53">
-        <v>541.5</v>
+        <v>594.9999999999999</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Örebro University</t>
+          <t>Uppsala University</t>
         </is>
       </c>
       <c r="B54">
-        <v>981</v>
-      </c>
-      <c r="C54">
-        <v>917</v>
+        <v>971</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Örebro University Hospital</t>
+          <t>Zealand University Hospital</t>
         </is>
       </c>
       <c r="B55">
-        <v>182</v>
+        <v>593.5</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>541.5</v>
       </c>
     </row>
     <row r="56">
@@ -1066,7 +1066,7 @@
         </is>
       </c>
       <c r="B57">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C57">
         <v>1508</v>
@@ -1105,7 +1105,7 @@
         <v>735.9999999999999</v>
       </c>
       <c r="C60">
-        <v>1217.000000000001</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="61">
@@ -1115,10 +1115,10 @@
         </is>
       </c>
       <c r="B61">
-        <v>698</v>
+        <v>697.5000000000001</v>
       </c>
       <c r="C61">
-        <v>1123</v>
+        <v>1123.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fix for one trial with wrong date
</commit_message>
<xml_diff>
--- a/data/3-analysis/output-results/tables/institution-median-rep-2023-11-28.xlsx
+++ b/data/3-analysis/output-results/tables/institution-median-rep-2023-11-28.xlsx
@@ -394,10 +394,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>793</v>
+        <v>652.0000000000001</v>
       </c>
       <c r="C3">
-        <v>758</v>
+        <v>712.0000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -407,10 +407,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="C4">
-        <v>834</v>
+        <v>821</v>
       </c>
     </row>
     <row r="5">
@@ -423,7 +423,7 @@
         <v>582</v>
       </c>
       <c r="C5">
-        <v>1133</v>
+        <v>884.0000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>631</v>
+        <v>623.9999999999999</v>
       </c>
       <c r="C7">
         <v>769</v>
@@ -462,7 +462,7 @@
         <v>722</v>
       </c>
       <c r="C8">
-        <v>1156.5</v>
+        <v>1052.5</v>
       </c>
     </row>
     <row r="9">
@@ -550,7 +550,7 @@
         <v>556</v>
       </c>
       <c r="C15">
-        <v>836.9999999999999</v>
+        <v>847.9999999999999</v>
       </c>
     </row>
     <row r="16">
@@ -677,7 +677,7 @@
         <v>892</v>
       </c>
       <c r="C25">
-        <v>1475.5</v>
+        <v>1456.5</v>
       </c>
     </row>
     <row r="26">
@@ -811,7 +811,7 @@
         </is>
       </c>
       <c r="B36">
-        <v>400.5000000000001</v>
+        <v>381.9999999999999</v>
       </c>
       <c r="C36">
         <v>734.0000000000001</v>
@@ -900,7 +900,7 @@
         </is>
       </c>
       <c r="B44">
-        <v>846</v>
+        <v>819</v>
       </c>
       <c r="C44">
         <v>1220</v>
@@ -1040,10 +1040,10 @@
         </is>
       </c>
       <c r="B55">
-        <v>593.5</v>
+        <v>594</v>
       </c>
       <c r="C55">
-        <v>541.5</v>
+        <v>529.4999999999999</v>
       </c>
     </row>
     <row r="56">
@@ -1053,10 +1053,10 @@
         </is>
       </c>
       <c r="B56">
-        <v>623.9999999999999</v>
+        <v>617</v>
       </c>
       <c r="C56">
-        <v>932.9999999999998</v>
+        <v>885.0000000000001</v>
       </c>
     </row>
     <row r="57">
@@ -1066,10 +1066,10 @@
         </is>
       </c>
       <c r="B57">
-        <v>720</v>
+        <v>702.5</v>
       </c>
       <c r="C57">
-        <v>1508</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="58">
@@ -1115,10 +1115,10 @@
         </is>
       </c>
       <c r="B61">
-        <v>697.5000000000001</v>
+        <v>690</v>
       </c>
       <c r="C61">
-        <v>1123.5</v>
+        <v>1103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>